<commit_message>
Advancing economy/business seat analysis and viz
</commit_message>
<xml_diff>
--- a/data/data_flight_economy_business.xlsx
+++ b/data/data_flight_economy_business.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/ls2823_ic_ac_uk/Documents/0_Sustainable Transport/COP_flight_analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="255" documentId="8_{2CF71990-6E5C-4EE8-BB14-F770DCE19548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F921BFF-8C9D-4D42-B447-A6BAA1271A67}"/>
+  <xr:revisionPtr revIDLastSave="331" documentId="8_{2CF71990-6E5C-4EE8-BB14-F770DCE19548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F33C84A9-11FD-40AF-97F3-FD21492844F5}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{40CED1EC-56BB-41F0-B509-74523F056A56}"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" activeTab="2" xr2:uid="{40CED1EC-56BB-41F0-B509-74523F056A56}"/>
   </bookViews>
   <sheets>
     <sheet name="direct" sheetId="1" r:id="rId1"/>
@@ -1287,7 +1287,13 @@
       <sheetName val="Non_Direct_new_hu"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>icao</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
@@ -2166,9 +2172,175 @@
             <v>0</v>
           </cell>
         </row>
+        <row r="45">
+          <cell r="A45" t="str">
+            <v>A312</v>
+          </cell>
+          <cell r="B45">
+            <v>345</v>
+          </cell>
+          <cell r="C45">
+            <v>66</v>
+          </cell>
+          <cell r="D45">
+            <v>279</v>
+          </cell>
+          <cell r="E45">
+            <v>544.6708860759494</v>
+          </cell>
+          <cell r="F45">
+            <v>0.19130434782608696</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="A46" t="str">
+            <v>B378</v>
+          </cell>
+          <cell r="B46">
+            <v>345</v>
+          </cell>
+          <cell r="C46">
+            <v>66</v>
+          </cell>
+          <cell r="D46">
+            <v>279</v>
+          </cell>
+          <cell r="E46">
+            <v>544.6708860759494</v>
+          </cell>
+          <cell r="F46">
+            <v>0.19130434782608696</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="A47" t="str">
+            <v>FA7X</v>
+          </cell>
+          <cell r="B47">
+            <v>345</v>
+          </cell>
+          <cell r="C47">
+            <v>66</v>
+          </cell>
+          <cell r="D47">
+            <v>279</v>
+          </cell>
+          <cell r="E47">
+            <v>544.6708860759494</v>
+          </cell>
+          <cell r="F47">
+            <v>0.19130434782608696</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="A48" t="str">
+            <v>E75S</v>
+          </cell>
+          <cell r="B48">
+            <v>345</v>
+          </cell>
+          <cell r="C48">
+            <v>66</v>
+          </cell>
+          <cell r="D48">
+            <v>279</v>
+          </cell>
+          <cell r="E48">
+            <v>544.6708860759494</v>
+          </cell>
+          <cell r="F48">
+            <v>0.19130434782608696</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="A49" t="str">
+            <v>A346</v>
+          </cell>
+          <cell r="B49">
+            <v>345</v>
+          </cell>
+          <cell r="C49">
+            <v>66</v>
+          </cell>
+          <cell r="D49">
+            <v>279</v>
+          </cell>
+          <cell r="E49">
+            <v>544.6708860759494</v>
+          </cell>
+          <cell r="F49">
+            <v>0.19130434782608696</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="A50" t="str">
+            <v>G280</v>
+          </cell>
+          <cell r="B50">
+            <v>345</v>
+          </cell>
+          <cell r="C50">
+            <v>66</v>
+          </cell>
+          <cell r="D50">
+            <v>279</v>
+          </cell>
+          <cell r="E50">
+            <v>544.6708860759494</v>
+          </cell>
+          <cell r="F50">
+            <v>0.19130434782608696</v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="A51" t="str">
+            <v>B739</v>
+          </cell>
+          <cell r="B51">
+            <v>345</v>
+          </cell>
+          <cell r="C51">
+            <v>66</v>
+          </cell>
+          <cell r="D51">
+            <v>279</v>
+          </cell>
+          <cell r="E51">
+            <v>544.6708860759494</v>
+          </cell>
+          <cell r="F51">
+            <v>0.19130434782608696</v>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="A52" t="str">
+            <v>A19N</v>
+          </cell>
+          <cell r="B52">
+            <v>345</v>
+          </cell>
+          <cell r="C52">
+            <v>66</v>
+          </cell>
+          <cell r="D52">
+            <v>279</v>
+          </cell>
+          <cell r="E52">
+            <v>544.6708860759494</v>
+          </cell>
+          <cell r="F52">
+            <v>0.19130434782608696</v>
+          </cell>
+        </row>
       </sheetData>
       <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
+      <sheetData sheetId="6">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>origin_airport</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="7"/>
       <sheetData sheetId="8"/>
     </sheetDataSet>
@@ -22810,8 +22982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B753E3F-A1F4-4E7F-82BF-CEC382F92E13}">
   <dimension ref="A1:R277"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59:XFD59"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -22828,7 +23000,7 @@
     <col min="16" max="16" width="13.453125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.1796875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">

</xml_diff>